<commit_message>
mini project code done 1
</commit_message>
<xml_diff>
--- a/Final.xlsx
+++ b/Final.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="MasterSheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MasterSheet11" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,6 +431,14 @@
       <c r="B1" t="n">
         <v>99003766</v>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>PS_NUMBER</t>
+        </is>
+      </c>
+      <c r="F1" t="n">
+        <v>99003754</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -443,6 +451,16 @@
           <t>Jayasimha Reddy Ganapuram</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Display Name</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Rishab Pankajkumar Ostawal</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -455,6 +473,16 @@
           <t>jayasimha.ganapuram@ltts.com</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Official Email Address</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>rishab.ostawal@ltts.com</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -467,6 +495,16 @@
           <t>Nalanda</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Training Hall</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Nalanda</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -477,6 +515,14 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Floor Number</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -489,6 +535,16 @@
           <t>8th feb,2021</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Date Of Joining</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>8th feb,2021</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -501,6 +557,16 @@
           <t>GT</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Domain</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>GT</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -513,6 +579,16 @@
           <t>Yes</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Attending Genesis</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -523,6 +599,14 @@
       <c r="B9" t="n">
         <v>21</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>System Number</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -533,6 +617,14 @@
       <c r="B10" t="n">
         <v>21</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Team Number</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -543,6 +635,14 @@
       <c r="B11" t="n">
         <v>2</v>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>BUS NUMBER</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -553,6 +653,14 @@
       <c r="B12" t="n">
         <v>9</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Working Hours</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -563,6 +671,14 @@
       <c r="B13" t="n">
         <v>60</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Marks Subject1</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -573,6 +689,14 @@
       <c r="B14" t="n">
         <v>63</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Marks Subject2</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -583,6 +707,14 @@
       <c r="B15" t="n">
         <v>55</v>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Marks Subject3</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -593,6 +725,14 @@
       <c r="B16" t="n">
         <v>37</v>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Marks Subject4</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -603,6 +743,14 @@
       <c r="B17" t="n">
         <v>53</v>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Marks Subject5</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -615,6 +763,16 @@
           <t>Pass</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -625,6 +783,14 @@
       <c r="B19" t="n">
         <v>40</v>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Number of clasess attended</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -635,6 +801,14 @@
       <c r="B20" t="n">
         <v>99</v>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ATTENDANCE </t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -647,6 +821,16 @@
           <t>Good</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Conduct</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -659,6 +843,16 @@
           <t>Fresher</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Experience</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Fresher</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -671,6 +865,16 @@
           <t>College</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Placement</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -681,6 +885,14 @@
       <c r="B24" t="n">
         <v>10000</v>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Salary </t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>10000</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -688,6 +900,11 @@
           <t>None</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -700,6 +917,16 @@
           <t>ECE</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Stream</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -712,6 +939,16 @@
           <t>Fairfield Marriot</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Fairfield Marriot</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -724,6 +961,16 @@
           <t>Rajajinagar</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Rajajinagar</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -734,6 +981,14 @@
       <c r="B29" t="n">
         <v>120</v>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Room Number</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>114</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -746,6 +1001,16 @@
           <t>AP</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Permanent Address</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>AP</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -756,6 +1021,14 @@
       <c r="B31" t="n">
         <v>21</v>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Data1</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -765,6 +1038,14 @@
       </c>
       <c r="B32" t="n">
         <v>120</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Data2</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final code mini project
</commit_message>
<xml_diff>
--- a/Final.xlsx
+++ b/Final.xlsx
@@ -123,6 +123,191 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t xml:space="preserve"> BAR-CHART </a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'MasterSheet11'!$B$9:$B$17</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'MasterSheet11'!$C$9:$C$17</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'MasterSheet11'!$D$9:$D$17</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'MasterSheet11'!$E$9:$E$17</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'MasterSheet11'!$F$9:$F$17</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t xml:space="preserve"> X_AXIS </a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t xml:space="preserve"> Y_AXIS </a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,7 +594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -437,7 +622,7 @@
         </is>
       </c>
       <c r="F1" t="n">
-        <v>99003754</v>
+        <v>99003737</v>
       </c>
     </row>
     <row r="2">
@@ -458,7 +643,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Rishab Pankajkumar Ostawal</t>
+          <t>Jeshwanth Kumar Ega</t>
         </is>
       </c>
     </row>
@@ -480,7 +665,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>rishab.ostawal@ltts.com</t>
+          <t>jeshwanth.ega@ltts.com</t>
         </is>
       </c>
     </row>
@@ -564,7 +749,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>SPS</t>
         </is>
       </c>
     </row>
@@ -605,7 +790,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +808,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -677,7 +862,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -695,7 +880,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -713,7 +898,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
@@ -749,7 +934,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
@@ -770,7 +955,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
     </row>
@@ -789,7 +974,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -807,7 +992,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -828,7 +1013,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>Very Bad</t>
         </is>
       </c>
     </row>
@@ -891,7 +1076,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>10000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -987,7 +1172,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>114</v>
+        <v>420</v>
       </c>
     </row>
     <row r="30">
@@ -1027,7 +1212,7 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
@@ -1045,11 +1230,12 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>